<commit_message>
changed excel file dir
</commit_message>
<xml_diff>
--- a/src/jobs_data.xlsx
+++ b/src/jobs_data.xlsx
@@ -473,88 +473,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Senior Front-End Developer (React) Remote</t>
+          <t>Remote Full-Stack Developer</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Uplers</t>
+          <t>Turing</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['$35K/yr', 'Remote', 'Full-time']</t>
+          <t>['Remote', 'Full-time']</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Reposted 3 days ago</t>
+          <t>Reposted 1 week ago</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
-        <is>
-          <t>*   Lead the development of cutting-edge web applications using React to improve user experiences.
-*   Collaborate closely with UI/UX designers to create accessible, intuitive, and visually appealing interfaces.
-*   Optimize performance using advanced React techniques (code-splitting, lazy loading, tree-shaking) to ensure fast load times and scalability.
-*   Integrate with RESTful, OData, and GraphQL APIs, ensuring seamless data flow and robust functionality.
-*   Mentor and guide junior developers, fostering a collaborative and innovative environment.
-*   Deploy React applications using Azure Static Web Apps, optimizing the deployment process via CI/CD pipelines in GitHub Actions.
-*   Continuously test and debug to ensure code quality and application stability.</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>*   6+ years of front-end development experience with React
-*   Strong proficiency in JavaScript (ES6+)
-*   HTML5
-*   CSS3
-*   State management tools (e.g., Redux, Context API)
-*   Git
-*   Webpack
-*   Component libraries (e.g., Material-UI, Tailwind CSS)
-*   Testing frameworks (e.g., Jest, Cypress)
-*   Building scalable, maintainable codebases
-*   TypeScript
-*   Server-side rendering (Next.js is a plus)
-*   Experience deploying web applications to Azure Static Web Apps
-*   OData services
-*   RESTful APIs
-*   GraphQL
-*   CI/CD pipelines (GitHub Actions)
-*   Micro-frontend architecture
-*   Docker
-*   Kubernetes
-*   Progressive Web Applications (PWA)</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/jobs/collections/recommended/?currentJobId=4291254013</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Remote Full-Stack Developer</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Turing</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>['Remote', 'Full-time']</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Reposted 1 week ago</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
         <is>
           <t>* Write clean, reusable, and maintainable code.
 * Participate in code reviews to ensure high-quality standards.
@@ -563,113 +500,175 @@
 * Deliver well-structured and documented code.</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>*   Strong JavaScript or TypeScript skills
+*   Bachelor’s or Master’s degree in Computer Science, Engineering, or equivalent experience
+*   Strong understanding of ES6 and frameworks like Node.js or React
+*   Knowledge of front-end, back-end, or full-stack development
+*   Interest in building scalable, secure web applications with clean architecture
+*   Good spoken and written communication skills in English
+*   Familiarity with additional frameworks like Vue.js, Angular, or Nest.js (Nice to have)
+*   Understanding of software quality assurance and test planning (Nice to have)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/collections/recommended/?currentJobId=4273383213</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Frontend Development Intern</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>IG Tech</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>['Remote', 'Internship']</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2 days ago</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>* Transform designs into functional, visually appealing web applications.
+* Build responsive layouts.
+* Improve user experiences.
+* Work with modern frameworks.</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>*   Open to applicants of all levels, from junior to industry experts.
-*   Bachelor’s or Master’s degree in Computer Science, Engineering, or equivalent experience.
-*   Strong understanding of ES6 and frameworks like Node.js or React.
-*   Knowledge of front-end, back-end, or full-stack development.
-*   Interest in building scalable, secure web applications with clean architecture.
-*   Good spoken and written communication skills in English.</t>
+          <t>*   Pursuing or recently completed a degree in Computer Science, IT, or related fields
+*   Proficiency in HTML, CSS, and JavaScript
+*   Familiarity with frameworks like React, Angular, or Vue
+*   Understanding of responsive design principles
+*   Basic knowledge of Git/GitHub for version control
+*   Creativity, problem-solving, and attention to detail</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/collections/recommended/?currentJobId=4273386039</t>
+          <t>https://www.linkedin.com/jobs/collections/recommended/?currentJobId=4300631848</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Senior Drupal &amp; PHP Developer with ASP.NET</t>
+          <t>Web Developer (Wordpress Fullstack Developer)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Braintrust</t>
+          <t>Uplers</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['Remote', 'Full-time']</t>
+          <t>['₹1.2M/yr - ₹1.8M/yr', 'Remote', 'Full-time']</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2 days ago</t>
+          <t>Reposted 2 weeks ago</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>* Develop and maintain applications using Drupal (latest version) and PHP.
-* Contribute to ASP.NET development with a minimum of 5 years of proven experience.
-* Support production Drupal platforms, especially those integrated with ASP.NET.
-* Participate in Drupal + PHP upgrade projects.
-* Customize PHP within Drupal to meet specific requirements.
-* Troubleshoot and resolve issues in Drupal + PHP production environments.
-* Collaborate with global teams during overlapping US Central Time working hours.</t>
+          <t>*   Design and implement modular, scalable front-end structures.
+*   Customize and extend CMS themes and components to meet project requirements.
+*   Write semantic, DRY, and well-organized HTML/CSS using naming conventions like BEM.
+*   Collaborate with designers, strategists, content, and SEO teams to bring digital concepts to life.
+*   Champion best practices and introduce efficiencies in development workflows.
+*   Deliver flexible and maintainable front-end codebases that support rapid updates and content scalability.
+*   Launch custom, fully editable CMS templates that balance design integrity with editorial flexibility.
+*   Implement changes based on technical SEO audits, ensuring site structure, performance, and markup align with search optimization best practices.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>* Minimum 2 years of hands-on development experience with Drupal &amp; PHP (latest version)
-* At least 5 years of experience with ASP.NET development
-* Prior experience in production Drupal environments
-* Experience in Drupal environments integrated with ASP.NET (preferred)
-* Strong problem-solving skills for production issue troubleshooting
-* Experience in Drupal + PHP upgrade projects (desirable)
-* Knowledge of other CMS systems (a plus)</t>
+          <t>*   3+ years of experience
+*   Proficiency in WordPress themes, Custom PHP (WordPress plugins), and WordPress integration
+*   Strong command of JavaScript and PHP
+*   Experience with workflow automation and other CMS
+*   Ability to architect scalable, reusable components and front-end structures
+*   Skilled in writing clean, maintainable, semantic, and DRY HTML/CSS using naming conventions (e.g., BEM), adhering to modern web standards
+*   Experience customizing and extending CMS themes and components
+*   Ability to champion best practices and introduce efficiencies in development workflows
+*   Systematic thinking for reusable patterns and scalable architecture
+*   Exceptional attention to detail (visual and functional fidelity)
+*   Strong technical communication skills (articulating decisions to non-developers)
+*   Proven collaboration skills with cross-functional teams (designers, strategists, content, SEO)
+*   Self-directed and proactive in problem-solving
+*   Code empathy (writing clean, logical, maintainable code)
+*   Adaptability to new tools, workflows, and CMS limitations
+*   Process-oriented approach to tasks and delivery
+*   User-focused mindset (considering end-user experience)
+*   SEO awareness (understanding impact on search performance, technical execution)
+*   Design sensitivity (executing visual design with precision)
+*   Mentorship mindset</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/collections/recommended/?currentJobId=4302104610</t>
+          <t>https://www.linkedin.com/jobs/collections/recommended/?currentJobId=4275329833</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[AS177] Senior PHP Laravel Developer (Remote, Full-Time)</t>
+          <t>Front End Development Intern</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Smart Working</t>
+          <t>PeopleOps Cloud</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['Remote', 'Full-time']</t>
+          <t>['Remote', 'Internship']</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2 weeks ago</t>
+          <t>4 days ago</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>*   Collaborate with the engineering team to complete backend projects using PHP and Laravel
-*   Troubleshoot and fix issues in PHP applications; identify root causes and verify fixes
-*   Design and implement greenfield systems with Laravel, writing clean and maintainable code
-*   Build and maintain RESTful APIs and integrations
-*   Use Git effectively (branching, pull requests, reviews) to support collaborative workflows</t>
+          <t>* Develop intuitive and scalable user interfaces for web applications.
+* Contribute to mobile app development using React Native.
+* Assist in designing and implementing conversational flows for chatbot solutions.
+* Collaborate with team members to deliver end-to-end product features.
+* Ensure UI/UX consistency and responsiveness across devices.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>*   Bachelor’s degree in Computer Science, Engineering, or a related discipline (or equivalent practical experience)
-*   4+ years of professional experience in software development
-*   PHP &amp; Laravel: 3+ years building production applications
-*   Working understanding of REST APIs, including design, debugging, and integration
-*   Proficiency with Git version control in collaborative development environments</t>
+          <t>*   Proficiency in React.js, React Native, JavaScript/TypeScript, HTML, and CSS.
+*   Basic understanding of UI/UX design principles.
+*   Familiarity with CSS frameworks (e.g., Bootstrap, Tailwind CSS).
+*   Knowledge of WhatsApp APIs or chatbot frameworks (Bonus).
+*   Strong problem-solving mindset and ability to work in a dynamic environment.
+*   Currently pursuing or recently completed a degree in Computer Science, Engineering, or a related field.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/collections/recommended/?currentJobId=4294471786</t>
+          <t>https://www.linkedin.com/jobs/collections/recommended/?currentJobId=4301397754</t>
         </is>
       </c>
     </row>

</xml_diff>